<commit_message>
chore: v0.3.1 release – focus dashboards, amount buckets, date parsing fixes, popover UX, bugfixes
</commit_message>
<xml_diff>
--- a/v1tracking_template.xlsx
+++ b/v1tracking_template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="286">
   <si>
     <t>市场国别</t>
   </si>
@@ -842,12 +842,24 @@
     <t>长庆钻总</t>
   </si>
   <si>
+    <t>秘鲁58区</t>
+  </si>
+  <si>
+    <t>58区修井</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>中石油秘鲁公司</t>
   </si>
   <si>
     <t>设备打包阶段，计划2025年11月15日集港，11月25日发运，2026年06月修井施工</t>
   </si>
   <si>
+    <t>长钻50090</t>
+  </si>
+  <si>
     <t>CCDC-87</t>
   </si>
   <si>
@@ -858,6 +870,24 @@
   </si>
   <si>
     <t>宝石146-2</t>
+  </si>
+  <si>
+    <t>CPOE</t>
+  </si>
+  <si>
+    <t>中油海工</t>
+  </si>
+  <si>
+    <t>AMISTAD项目</t>
+  </si>
+  <si>
+    <t>海上修井</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>目前：整改设备，作业前准备，配合甲方测试设备，配钻具。</t>
   </si>
 </sst>
 </file>
@@ -2619,10 +2649,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V51"/>
+  <dimension ref="A1:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="D33" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -5102,20 +5132,29 @@
       <c r="I50" s="68" t="s">
         <v>269</v>
       </c>
-      <c r="J50" s="145"/>
-      <c r="K50" s="145"/>
+      <c r="J50" s="145" t="s">
+        <v>270</v>
+      </c>
+      <c r="K50" s="145" t="s">
+        <v>271</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="P50" s="75" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="Q50" s="150" t="s">
         <v>43</v>
       </c>
       <c r="R50" s="139" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="S50" s="139"/>
       <c r="T50" s="139"/>
-      <c r="V50" s="95"/>
+      <c r="V50" s="95" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="51" ht="50.25" spans="1:22">
       <c r="A51" t="s">
@@ -5125,10 +5164,10 @@
         <v>14</v>
       </c>
       <c r="C51" s="152" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="E51" s="152"/>
       <c r="F51" s="153" t="s">
@@ -5152,12 +5191,44 @@
         <v>43</v>
       </c>
       <c r="R51" s="156" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="S51" s="157"/>
       <c r="T51" s="157"/>
       <c r="V51" s="95" t="s">
-        <v>275</v>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22">
+      <c r="A52" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52">
+        <v>15</v>
+      </c>
+      <c r="C52" t="s">
+        <v>280</v>
+      </c>
+      <c r="I52" t="s">
+        <v>281</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R52" t="s">
+        <v>285</v>
+      </c>
+      <c r="V52" s="4" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>